<commit_message>
Modify Sample Transfer submission template
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_transfer_v0.1.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_transfer_v0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jleblond/c3g/freezeman/backend/fms_core/static/submission_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB03ECC-1AF0-6C4E-B815-4A2F811508C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374277ED-53E1-7D4A-B985-983F7CCF7A88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36300" yWindow="3860" windowWidth="28800" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34200" yWindow="5300" windowWidth="28800" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleTransferTemplate" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="405">
   <si>
     <t>#</t>
   </si>
@@ -1222,55 +1222,25 @@
     <t>Destination Parent Container Barcode</t>
   </si>
   <si>
-    <t>Destination Parent Location Coord</t>
-  </si>
-  <si>
     <t>Destination Container Name</t>
   </si>
   <si>
     <t>Destination Container Kind</t>
   </si>
   <si>
-    <t>Tube box 8x8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tube box 9x9 </t>
-  </si>
-  <si>
-    <t>Tube box 10x10</t>
-  </si>
-  <si>
-    <t>Tube rack 8x12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drawer </t>
-  </si>
-  <si>
-    <t>Freezer rack 4x4</t>
-  </si>
-  <si>
-    <t>Freezer rack 7x4</t>
-  </si>
-  <si>
-    <t>Freezer rack 8x6</t>
-  </si>
-  <si>
-    <t>Freezer rack 11x6</t>
-  </si>
-  <si>
-    <t>Freezer 3 shelves</t>
-  </si>
-  <si>
-    <t>Freezer 5 shelves</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
     <t>Source Depleted</t>
+  </si>
+  <si>
+    <t>Tube</t>
+  </si>
+  <si>
+    <t>96-well plate</t>
+  </si>
+  <si>
+    <t>384-well plate</t>
+  </si>
+  <si>
+    <t>Destination Parent Container Coord</t>
   </si>
 </sst>
 </file>
@@ -1599,122 +1569,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="slantDashDot">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="slantDashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="slantDashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="slantDashDot">
-        <color indexed="64"/>
-      </right>
-      <top style="slantDashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="slantDashDot">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="slantDashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="slantDashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="mediumDashed">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="slantDashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="mediumDashed">
         <color indexed="64"/>
       </left>
@@ -1739,7 +1593,121 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="slantDashDot">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1806,31 +1774,29 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2228,12 +2194,12 @@
     <col min="5" max="5" width="26.1640625" customWidth="1"/>
     <col min="6" max="6" width="25.5" customWidth="1"/>
     <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="33.5" customWidth="1"/>
-    <col min="9" max="9" width="28.83203125" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="17.1640625" customWidth="1"/>
-    <col min="12" max="13" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="29" customWidth="1"/>
+    <col min="8" max="9" width="33.5" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16.5" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="38.33203125" customWidth="1"/>
     <col min="15" max="30" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2278,26 +2244,26 @@
       <c r="C8" s="8" t="s">
         <v>392</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="37" t="s">
         <v>393</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>394</v>
       </c>
       <c r="F8" s="32" t="s">
+        <v>398</v>
+      </c>
+      <c r="G8" s="38" t="s">
         <v>399</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="H8" s="39" t="s">
+        <v>397</v>
+      </c>
+      <c r="I8" s="40" t="s">
+        <v>404</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>400</v>
-      </c>
-      <c r="H8" s="38" t="s">
-        <v>397</v>
-      </c>
-      <c r="I8" s="33" t="s">
-        <v>398</v>
-      </c>
-      <c r="J8" s="43" t="s">
-        <v>414</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>1</v>
@@ -2317,14 +2283,14 @@
         <v>1</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="29"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="34"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="26"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="23"/>
       <c r="K9" s="23"/>
       <c r="L9" s="10"/>
       <c r="M9" s="16"/>
@@ -2336,13 +2302,13 @@
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="21"/>
-      <c r="D10" s="30"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="26"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="10"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="23"/>
       <c r="K10" s="24"/>
       <c r="L10" s="11"/>
       <c r="M10" s="16"/>
@@ -2354,13 +2320,13 @@
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="21"/>
-      <c r="D11" s="30"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="26"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="10"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="23"/>
       <c r="K11" s="24"/>
       <c r="L11" s="11"/>
       <c r="M11" s="16"/>
@@ -2372,13 +2338,13 @@
       </c>
       <c r="B12" s="11"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
       <c r="G12" s="26"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="10"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="23"/>
       <c r="K12" s="24"/>
       <c r="L12" s="11"/>
       <c r="M12" s="16"/>
@@ -2390,13 +2356,13 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="30"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="26"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="10"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="23"/>
       <c r="K13" s="24"/>
       <c r="L13" s="11"/>
       <c r="M13" s="16"/>
@@ -2408,13 +2374,13 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="30"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
       <c r="G14" s="26"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="10"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="23"/>
       <c r="K14" s="24"/>
       <c r="L14" s="11"/>
       <c r="M14" s="16"/>
@@ -2426,13 +2392,13 @@
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="30"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
       <c r="G15" s="26"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="10"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="23"/>
       <c r="K15" s="24"/>
       <c r="L15" s="11"/>
       <c r="M15" s="16"/>
@@ -2444,13 +2410,13 @@
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="26"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="10"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="24"/>
       <c r="L16" s="11"/>
       <c r="M16" s="16"/>
@@ -2462,13 +2428,13 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="21"/>
-      <c r="D17" s="30"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
       <c r="G17" s="26"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="10"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="24"/>
       <c r="L17" s="11"/>
       <c r="M17" s="16"/>
@@ -2480,13 +2446,13 @@
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="30"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
       <c r="G18" s="26"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="10"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="23"/>
       <c r="K18" s="24"/>
       <c r="L18" s="11"/>
       <c r="M18" s="16"/>
@@ -2498,13 +2464,13 @@
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="30"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
       <c r="G19" s="26"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="10"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="23"/>
       <c r="K19" s="24"/>
       <c r="L19" s="11"/>
       <c r="M19" s="16"/>
@@ -2516,13 +2482,13 @@
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="30"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="10"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="23"/>
       <c r="K20" s="24"/>
       <c r="L20" s="11"/>
       <c r="M20" s="16"/>
@@ -2534,13 +2500,13 @@
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="21"/>
-      <c r="D21" s="30"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
       <c r="G21" s="26"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="10"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="23"/>
       <c r="K21" s="24"/>
       <c r="L21" s="11"/>
       <c r="M21" s="16"/>
@@ -2552,13 +2518,13 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="30"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
       <c r="G22" s="26"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="10"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="23"/>
       <c r="K22" s="24"/>
       <c r="L22" s="11"/>
       <c r="M22" s="16"/>
@@ -2570,13 +2536,13 @@
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="30"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="11"/>
       <c r="F23" s="11"/>
       <c r="G23" s="26"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="10"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="23"/>
       <c r="K23" s="24"/>
       <c r="L23" s="11"/>
       <c r="M23" s="16"/>
@@ -2588,13 +2554,13 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="30"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="26"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="10"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="23"/>
       <c r="K24" s="24"/>
       <c r="L24" s="11"/>
       <c r="M24" s="16"/>
@@ -2606,13 +2572,13 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="30"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="26"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="10"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="23"/>
       <c r="K25" s="24"/>
       <c r="L25" s="11"/>
       <c r="M25" s="16"/>
@@ -2624,13 +2590,13 @@
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="21"/>
-      <c r="D26" s="30"/>
+      <c r="D26" s="35"/>
       <c r="E26" s="11"/>
       <c r="F26" s="11"/>
       <c r="G26" s="26"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="10"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="23"/>
       <c r="K26" s="24"/>
       <c r="L26" s="11"/>
       <c r="M26" s="16"/>
@@ -2642,13 +2608,13 @@
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="21"/>
-      <c r="D27" s="30"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="26"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="10"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="23"/>
       <c r="K27" s="24"/>
       <c r="L27" s="11"/>
       <c r="M27" s="16"/>
@@ -2660,13 +2626,13 @@
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="21"/>
-      <c r="D28" s="30"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="26"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="10"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="23"/>
       <c r="K28" s="24"/>
       <c r="L28" s="11"/>
       <c r="M28" s="16"/>
@@ -2678,13 +2644,13 @@
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="21"/>
-      <c r="D29" s="30"/>
+      <c r="D29" s="35"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="26"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="10"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="23"/>
       <c r="K29" s="24"/>
       <c r="L29" s="11"/>
       <c r="M29" s="16"/>
@@ -2696,13 +2662,13 @@
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="30"/>
+      <c r="D30" s="35"/>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
       <c r="G30" s="26"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="10"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="23"/>
       <c r="K30" s="24"/>
       <c r="L30" s="11"/>
       <c r="M30" s="16"/>
@@ -2714,13 +2680,13 @@
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="30"/>
+      <c r="D31" s="35"/>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
       <c r="G31" s="26"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="10"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="23"/>
       <c r="K31" s="24"/>
       <c r="L31" s="11"/>
       <c r="M31" s="16"/>
@@ -2732,13 +2698,13 @@
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="30"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="11"/>
       <c r="F32" s="11"/>
       <c r="G32" s="26"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="10"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="23"/>
       <c r="K32" s="24"/>
       <c r="L32" s="11"/>
       <c r="M32" s="16"/>
@@ -2750,13 +2716,13 @@
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="30"/>
+      <c r="D33" s="35"/>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="26"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="10"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="23"/>
       <c r="K33" s="24"/>
       <c r="L33" s="11"/>
       <c r="M33" s="16"/>
@@ -2768,13 +2734,13 @@
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="30"/>
+      <c r="D34" s="35"/>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="26"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="10"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="23"/>
       <c r="K34" s="24"/>
       <c r="L34" s="11"/>
       <c r="M34" s="16"/>
@@ -2786,13 +2752,13 @@
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="21"/>
-      <c r="D35" s="30"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="26"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="10"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="41"/>
+      <c r="J35" s="23"/>
       <c r="K35" s="24"/>
       <c r="L35" s="11"/>
       <c r="M35" s="16"/>
@@ -2804,13 +2770,13 @@
       </c>
       <c r="B36" s="11"/>
       <c r="C36" s="21"/>
-      <c r="D36" s="30"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="26"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="10"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="23"/>
       <c r="K36" s="24"/>
       <c r="L36" s="11"/>
       <c r="M36" s="16"/>
@@ -2822,13 +2788,13 @@
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="21"/>
-      <c r="D37" s="30"/>
+      <c r="D37" s="35"/>
       <c r="E37" s="11"/>
       <c r="F37" s="11"/>
       <c r="G37" s="26"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="10"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="23"/>
       <c r="K37" s="24"/>
       <c r="L37" s="11"/>
       <c r="M37" s="16"/>
@@ -2840,13 +2806,13 @@
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="21"/>
-      <c r="D38" s="30"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="11"/>
       <c r="F38" s="11"/>
       <c r="G38" s="26"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="10"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="23"/>
       <c r="K38" s="24"/>
       <c r="L38" s="11"/>
       <c r="M38" s="16"/>
@@ -2858,13 +2824,13 @@
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="21"/>
-      <c r="D39" s="30"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="26"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="10"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="23"/>
       <c r="K39" s="24"/>
       <c r="L39" s="11"/>
       <c r="M39" s="16"/>
@@ -2876,13 +2842,13 @@
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="21"/>
-      <c r="D40" s="30"/>
+      <c r="D40" s="35"/>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
       <c r="G40" s="26"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="10"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="41"/>
+      <c r="J40" s="23"/>
       <c r="K40" s="24"/>
       <c r="L40" s="11"/>
       <c r="M40" s="16"/>
@@ -2894,13 +2860,13 @@
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="21"/>
-      <c r="D41" s="30"/>
+      <c r="D41" s="35"/>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
       <c r="G41" s="26"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="10"/>
+      <c r="H41" s="30"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="23"/>
       <c r="K41" s="24"/>
       <c r="L41" s="11"/>
       <c r="M41" s="16"/>
@@ -2912,13 +2878,13 @@
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="21"/>
-      <c r="D42" s="30"/>
+      <c r="D42" s="35"/>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
       <c r="G42" s="26"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="10"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="23"/>
       <c r="K42" s="24"/>
       <c r="L42" s="11"/>
       <c r="M42" s="16"/>
@@ -2930,13 +2896,13 @@
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="21"/>
-      <c r="D43" s="30"/>
+      <c r="D43" s="35"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
       <c r="G43" s="26"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="10"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="23"/>
       <c r="K43" s="24"/>
       <c r="L43" s="11"/>
       <c r="M43" s="16"/>
@@ -2948,13 +2914,13 @@
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="21"/>
-      <c r="D44" s="30"/>
+      <c r="D44" s="35"/>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="10"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="23"/>
       <c r="K44" s="24"/>
       <c r="L44" s="11"/>
       <c r="M44" s="16"/>
@@ -2966,13 +2932,13 @@
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="21"/>
-      <c r="D45" s="30"/>
+      <c r="D45" s="35"/>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="10"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="23"/>
       <c r="K45" s="24"/>
       <c r="L45" s="11"/>
       <c r="M45" s="16"/>
@@ -2984,13 +2950,13 @@
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="21"/>
-      <c r="D46" s="30"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="26"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="10"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="23"/>
       <c r="K46" s="24"/>
       <c r="L46" s="11"/>
       <c r="M46" s="16"/>
@@ -3002,13 +2968,13 @@
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="21"/>
-      <c r="D47" s="30"/>
+      <c r="D47" s="35"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="10"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="23"/>
       <c r="K47" s="24"/>
       <c r="L47" s="11"/>
       <c r="M47" s="16"/>
@@ -3020,13 +2986,13 @@
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="21"/>
-      <c r="D48" s="30"/>
+      <c r="D48" s="35"/>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="26"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="10"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="23"/>
       <c r="K48" s="24"/>
       <c r="L48" s="11"/>
       <c r="M48" s="16"/>
@@ -3038,13 +3004,13 @@
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="21"/>
-      <c r="D49" s="30"/>
+      <c r="D49" s="35"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="26"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="10"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="23"/>
       <c r="K49" s="24"/>
       <c r="L49" s="11"/>
       <c r="M49" s="16"/>
@@ -3056,13 +3022,13 @@
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="21"/>
-      <c r="D50" s="30"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="26"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="10"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="23"/>
       <c r="K50" s="24"/>
       <c r="L50" s="11"/>
       <c r="M50" s="16"/>
@@ -3074,13 +3040,13 @@
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="21"/>
-      <c r="D51" s="30"/>
+      <c r="D51" s="35"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
       <c r="G51" s="26"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="10"/>
+      <c r="H51" s="30"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="23"/>
       <c r="K51" s="24"/>
       <c r="L51" s="11"/>
       <c r="M51" s="16"/>
@@ -3092,13 +3058,13 @@
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="21"/>
-      <c r="D52" s="30"/>
+      <c r="D52" s="35"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="26"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="10"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="23"/>
       <c r="K52" s="24"/>
       <c r="L52" s="11"/>
       <c r="M52" s="16"/>
@@ -3110,13 +3076,13 @@
       </c>
       <c r="B53" s="11"/>
       <c r="C53" s="21"/>
-      <c r="D53" s="30"/>
+      <c r="D53" s="35"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="26"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="10"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="23"/>
       <c r="K53" s="24"/>
       <c r="L53" s="11"/>
       <c r="M53" s="16"/>
@@ -3128,13 +3094,13 @@
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="21"/>
-      <c r="D54" s="30"/>
+      <c r="D54" s="35"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
       <c r="G54" s="26"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="10"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="23"/>
       <c r="K54" s="24"/>
       <c r="L54" s="11"/>
       <c r="M54" s="16"/>
@@ -3146,13 +3112,13 @@
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="21"/>
-      <c r="D55" s="30"/>
+      <c r="D55" s="35"/>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
       <c r="G55" s="26"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="10"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="41"/>
+      <c r="J55" s="23"/>
       <c r="K55" s="24"/>
       <c r="L55" s="11"/>
       <c r="M55" s="16"/>
@@ -3164,13 +3130,13 @@
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="21"/>
-      <c r="D56" s="30"/>
+      <c r="D56" s="35"/>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
       <c r="G56" s="26"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="10"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="23"/>
       <c r="K56" s="24"/>
       <c r="L56" s="11"/>
       <c r="M56" s="16"/>
@@ -3182,13 +3148,13 @@
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="21"/>
-      <c r="D57" s="30"/>
+      <c r="D57" s="35"/>
       <c r="E57" s="11"/>
       <c r="F57" s="11"/>
       <c r="G57" s="26"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="10"/>
+      <c r="H57" s="30"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="23"/>
       <c r="K57" s="24"/>
       <c r="L57" s="11"/>
       <c r="M57" s="16"/>
@@ -3200,13 +3166,13 @@
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="21"/>
-      <c r="D58" s="30"/>
+      <c r="D58" s="35"/>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
       <c r="G58" s="26"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="10"/>
+      <c r="H58" s="30"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="23"/>
       <c r="K58" s="24"/>
       <c r="L58" s="11"/>
       <c r="M58" s="16"/>
@@ -3218,13 +3184,13 @@
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="21"/>
-      <c r="D59" s="30"/>
+      <c r="D59" s="35"/>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
       <c r="G59" s="26"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="10"/>
+      <c r="H59" s="30"/>
+      <c r="I59" s="41"/>
+      <c r="J59" s="23"/>
       <c r="K59" s="24"/>
       <c r="L59" s="11"/>
       <c r="M59" s="16"/>
@@ -3236,13 +3202,13 @@
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="21"/>
-      <c r="D60" s="30"/>
+      <c r="D60" s="35"/>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
       <c r="G60" s="26"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="10"/>
+      <c r="H60" s="30"/>
+      <c r="I60" s="41"/>
+      <c r="J60" s="23"/>
       <c r="K60" s="24"/>
       <c r="L60" s="11"/>
       <c r="M60" s="16"/>
@@ -3254,13 +3220,13 @@
       </c>
       <c r="B61" s="11"/>
       <c r="C61" s="21"/>
-      <c r="D61" s="30"/>
+      <c r="D61" s="35"/>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
       <c r="G61" s="26"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="10"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="41"/>
+      <c r="J61" s="23"/>
       <c r="K61" s="24"/>
       <c r="L61" s="11"/>
       <c r="M61" s="16"/>
@@ -3272,13 +3238,13 @@
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="21"/>
-      <c r="D62" s="30"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
       <c r="G62" s="26"/>
-      <c r="H62" s="40"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="10"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="41"/>
+      <c r="J62" s="23"/>
       <c r="K62" s="24"/>
       <c r="L62" s="11"/>
       <c r="M62" s="16"/>
@@ -3290,13 +3256,13 @@
       </c>
       <c r="B63" s="11"/>
       <c r="C63" s="21"/>
-      <c r="D63" s="30"/>
+      <c r="D63" s="35"/>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
       <c r="G63" s="26"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="10"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="41"/>
+      <c r="J63" s="23"/>
       <c r="K63" s="24"/>
       <c r="L63" s="11"/>
       <c r="M63" s="16"/>
@@ -3308,13 +3274,13 @@
       </c>
       <c r="B64" s="11"/>
       <c r="C64" s="21"/>
-      <c r="D64" s="30"/>
+      <c r="D64" s="35"/>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
       <c r="G64" s="27"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="10"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="41"/>
+      <c r="J64" s="23"/>
       <c r="K64" s="24"/>
       <c r="L64" s="11"/>
       <c r="M64" s="16"/>
@@ -3326,13 +3292,13 @@
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="21"/>
-      <c r="D65" s="30"/>
+      <c r="D65" s="35"/>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
       <c r="G65" s="27"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="10"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="41"/>
+      <c r="J65" s="23"/>
       <c r="K65" s="24"/>
       <c r="L65" s="11"/>
       <c r="M65" s="16"/>
@@ -3344,13 +3310,13 @@
       </c>
       <c r="B66" s="11"/>
       <c r="C66" s="21"/>
-      <c r="D66" s="30"/>
+      <c r="D66" s="35"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="27"/>
-      <c r="H66" s="40"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="10"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="23"/>
       <c r="K66" s="24"/>
       <c r="L66" s="11"/>
       <c r="M66" s="16"/>
@@ -3362,13 +3328,13 @@
       </c>
       <c r="B67" s="11"/>
       <c r="C67" s="21"/>
-      <c r="D67" s="30"/>
+      <c r="D67" s="35"/>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
       <c r="G67" s="27"/>
-      <c r="H67" s="40"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="10"/>
+      <c r="H67" s="30"/>
+      <c r="I67" s="41"/>
+      <c r="J67" s="23"/>
       <c r="K67" s="24"/>
       <c r="L67" s="11"/>
       <c r="M67" s="16"/>
@@ -3380,13 +3346,13 @@
       </c>
       <c r="B68" s="11"/>
       <c r="C68" s="21"/>
-      <c r="D68" s="30"/>
+      <c r="D68" s="35"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
       <c r="G68" s="28"/>
-      <c r="H68" s="40"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="10"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="41"/>
+      <c r="J68" s="23"/>
       <c r="K68" s="24"/>
       <c r="L68" s="11"/>
       <c r="M68" s="16"/>
@@ -3398,13 +3364,13 @@
       </c>
       <c r="B69" s="11"/>
       <c r="C69" s="21"/>
-      <c r="D69" s="30"/>
+      <c r="D69" s="35"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
       <c r="G69" s="27"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="10"/>
+      <c r="H69" s="30"/>
+      <c r="I69" s="41"/>
+      <c r="J69" s="23"/>
       <c r="K69" s="24"/>
       <c r="L69" s="11"/>
       <c r="M69" s="16"/>
@@ -3416,13 +3382,13 @@
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="21"/>
-      <c r="D70" s="30"/>
+      <c r="D70" s="35"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
       <c r="G70" s="27"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="10"/>
+      <c r="H70" s="30"/>
+      <c r="I70" s="41"/>
+      <c r="J70" s="23"/>
       <c r="K70" s="24"/>
       <c r="L70" s="11"/>
       <c r="M70" s="16"/>
@@ -3434,13 +3400,13 @@
       </c>
       <c r="B71" s="11"/>
       <c r="C71" s="21"/>
-      <c r="D71" s="30"/>
+      <c r="D71" s="35"/>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
       <c r="G71" s="27"/>
-      <c r="H71" s="40"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="10"/>
+      <c r="H71" s="30"/>
+      <c r="I71" s="41"/>
+      <c r="J71" s="23"/>
       <c r="K71" s="24"/>
       <c r="L71" s="11"/>
       <c r="M71" s="16"/>
@@ -3452,13 +3418,13 @@
       </c>
       <c r="B72" s="11"/>
       <c r="C72" s="21"/>
-      <c r="D72" s="30"/>
+      <c r="D72" s="35"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
       <c r="G72" s="27"/>
-      <c r="H72" s="40"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="10"/>
+      <c r="H72" s="30"/>
+      <c r="I72" s="41"/>
+      <c r="J72" s="23"/>
       <c r="K72" s="24"/>
       <c r="L72" s="11"/>
       <c r="M72" s="16"/>
@@ -3470,13 +3436,13 @@
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="21"/>
-      <c r="D73" s="30"/>
+      <c r="D73" s="35"/>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
       <c r="G73" s="27"/>
-      <c r="H73" s="40"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="10"/>
+      <c r="H73" s="30"/>
+      <c r="I73" s="41"/>
+      <c r="J73" s="23"/>
       <c r="K73" s="24"/>
       <c r="L73" s="11"/>
       <c r="M73" s="16"/>
@@ -3488,13 +3454,13 @@
       </c>
       <c r="B74" s="11"/>
       <c r="C74" s="21"/>
-      <c r="D74" s="30"/>
+      <c r="D74" s="35"/>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
       <c r="G74" s="27"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="10"/>
+      <c r="H74" s="30"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="23"/>
       <c r="K74" s="24"/>
       <c r="L74" s="11"/>
       <c r="M74" s="16"/>
@@ -3506,13 +3472,13 @@
       </c>
       <c r="B75" s="11"/>
       <c r="C75" s="21"/>
-      <c r="D75" s="30"/>
+      <c r="D75" s="35"/>
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
       <c r="G75" s="27"/>
-      <c r="H75" s="40"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="10"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="41"/>
+      <c r="J75" s="23"/>
       <c r="K75" s="24"/>
       <c r="L75" s="11"/>
       <c r="M75" s="16"/>
@@ -3524,13 +3490,13 @@
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="21"/>
-      <c r="D76" s="30"/>
+      <c r="D76" s="35"/>
       <c r="E76" s="11"/>
       <c r="F76" s="11"/>
       <c r="G76" s="27"/>
-      <c r="H76" s="40"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="10"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="41"/>
+      <c r="J76" s="23"/>
       <c r="K76" s="24"/>
       <c r="L76" s="11"/>
       <c r="M76" s="16"/>
@@ -3542,13 +3508,13 @@
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="21"/>
-      <c r="D77" s="30"/>
+      <c r="D77" s="35"/>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
       <c r="G77" s="27"/>
-      <c r="H77" s="40"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="10"/>
+      <c r="H77" s="30"/>
+      <c r="I77" s="41"/>
+      <c r="J77" s="23"/>
       <c r="K77" s="24"/>
       <c r="L77" s="11"/>
       <c r="M77" s="16"/>
@@ -3560,13 +3526,13 @@
       </c>
       <c r="B78" s="11"/>
       <c r="C78" s="21"/>
-      <c r="D78" s="30"/>
+      <c r="D78" s="35"/>
       <c r="E78" s="11"/>
       <c r="F78" s="11"/>
       <c r="G78" s="28"/>
-      <c r="H78" s="40"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="10"/>
+      <c r="H78" s="30"/>
+      <c r="I78" s="41"/>
+      <c r="J78" s="23"/>
       <c r="K78" s="24"/>
       <c r="L78" s="11"/>
       <c r="M78" s="16"/>
@@ -3578,13 +3544,13 @@
       </c>
       <c r="B79" s="11"/>
       <c r="C79" s="21"/>
-      <c r="D79" s="30"/>
+      <c r="D79" s="35"/>
       <c r="E79" s="11"/>
       <c r="F79" s="11"/>
       <c r="G79" s="27"/>
-      <c r="H79" s="40"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="10"/>
+      <c r="H79" s="30"/>
+      <c r="I79" s="41"/>
+      <c r="J79" s="23"/>
       <c r="K79" s="24"/>
       <c r="L79" s="11"/>
       <c r="M79" s="16"/>
@@ -3596,13 +3562,13 @@
       </c>
       <c r="B80" s="11"/>
       <c r="C80" s="21"/>
-      <c r="D80" s="30"/>
+      <c r="D80" s="35"/>
       <c r="E80" s="11"/>
       <c r="F80" s="11"/>
       <c r="G80" s="27"/>
-      <c r="H80" s="40"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="10"/>
+      <c r="H80" s="30"/>
+      <c r="I80" s="41"/>
+      <c r="J80" s="23"/>
       <c r="K80" s="24"/>
       <c r="L80" s="11"/>
       <c r="M80" s="16"/>
@@ -3614,13 +3580,13 @@
       </c>
       <c r="B81" s="11"/>
       <c r="C81" s="21"/>
-      <c r="D81" s="30"/>
+      <c r="D81" s="35"/>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
       <c r="G81" s="27"/>
-      <c r="H81" s="40"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="10"/>
+      <c r="H81" s="30"/>
+      <c r="I81" s="41"/>
+      <c r="J81" s="23"/>
       <c r="K81" s="24"/>
       <c r="L81" s="11"/>
       <c r="M81" s="16"/>
@@ -3632,13 +3598,13 @@
       </c>
       <c r="B82" s="11"/>
       <c r="C82" s="21"/>
-      <c r="D82" s="30"/>
+      <c r="D82" s="35"/>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
       <c r="G82" s="27"/>
-      <c r="H82" s="40"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="10"/>
+      <c r="H82" s="30"/>
+      <c r="I82" s="41"/>
+      <c r="J82" s="23"/>
       <c r="K82" s="24"/>
       <c r="L82" s="11"/>
       <c r="M82" s="16"/>
@@ -3650,13 +3616,13 @@
       </c>
       <c r="B83" s="11"/>
       <c r="C83" s="21"/>
-      <c r="D83" s="30"/>
+      <c r="D83" s="35"/>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
       <c r="G83" s="27"/>
-      <c r="H83" s="40"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="10"/>
+      <c r="H83" s="30"/>
+      <c r="I83" s="41"/>
+      <c r="J83" s="23"/>
       <c r="K83" s="24"/>
       <c r="L83" s="11"/>
       <c r="M83" s="16"/>
@@ -3668,13 +3634,13 @@
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="21"/>
-      <c r="D84" s="30"/>
+      <c r="D84" s="35"/>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
       <c r="G84" s="27"/>
-      <c r="H84" s="40"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="10"/>
+      <c r="H84" s="30"/>
+      <c r="I84" s="41"/>
+      <c r="J84" s="23"/>
       <c r="K84" s="24"/>
       <c r="L84" s="11"/>
       <c r="M84" s="16"/>
@@ -3686,13 +3652,13 @@
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="21"/>
-      <c r="D85" s="30"/>
+      <c r="D85" s="35"/>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
       <c r="G85" s="27"/>
-      <c r="H85" s="40"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="10"/>
+      <c r="H85" s="30"/>
+      <c r="I85" s="41"/>
+      <c r="J85" s="23"/>
       <c r="K85" s="24"/>
       <c r="L85" s="11"/>
       <c r="M85" s="16"/>
@@ -3704,13 +3670,13 @@
       </c>
       <c r="B86" s="11"/>
       <c r="C86" s="21"/>
-      <c r="D86" s="30"/>
+      <c r="D86" s="35"/>
       <c r="E86" s="11"/>
       <c r="F86" s="11"/>
       <c r="G86" s="27"/>
-      <c r="H86" s="40"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="10"/>
+      <c r="H86" s="30"/>
+      <c r="I86" s="41"/>
+      <c r="J86" s="23"/>
       <c r="K86" s="24"/>
       <c r="L86" s="11"/>
       <c r="M86" s="16"/>
@@ -3722,13 +3688,13 @@
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="21"/>
-      <c r="D87" s="30"/>
+      <c r="D87" s="35"/>
       <c r="E87" s="11"/>
       <c r="F87" s="11"/>
       <c r="G87" s="27"/>
-      <c r="H87" s="40"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="10"/>
+      <c r="H87" s="30"/>
+      <c r="I87" s="41"/>
+      <c r="J87" s="23"/>
       <c r="K87" s="24"/>
       <c r="L87" s="11"/>
       <c r="M87" s="16"/>
@@ -3740,13 +3706,13 @@
       </c>
       <c r="B88" s="11"/>
       <c r="C88" s="21"/>
-      <c r="D88" s="30"/>
+      <c r="D88" s="35"/>
       <c r="E88" s="11"/>
       <c r="F88" s="11"/>
       <c r="G88" s="28"/>
-      <c r="H88" s="40"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="10"/>
+      <c r="H88" s="30"/>
+      <c r="I88" s="41"/>
+      <c r="J88" s="23"/>
       <c r="K88" s="24"/>
       <c r="L88" s="11"/>
       <c r="M88" s="16"/>
@@ -3758,13 +3724,13 @@
       </c>
       <c r="B89" s="11"/>
       <c r="C89" s="21"/>
-      <c r="D89" s="30"/>
+      <c r="D89" s="35"/>
       <c r="E89" s="11"/>
       <c r="F89" s="11"/>
       <c r="G89" s="27"/>
-      <c r="H89" s="40"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="10"/>
+      <c r="H89" s="30"/>
+      <c r="I89" s="41"/>
+      <c r="J89" s="23"/>
       <c r="K89" s="24"/>
       <c r="L89" s="11"/>
       <c r="M89" s="16"/>
@@ -3776,13 +3742,13 @@
       </c>
       <c r="B90" s="11"/>
       <c r="C90" s="21"/>
-      <c r="D90" s="30"/>
+      <c r="D90" s="35"/>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
       <c r="G90" s="27"/>
-      <c r="H90" s="40"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="10"/>
+      <c r="H90" s="30"/>
+      <c r="I90" s="41"/>
+      <c r="J90" s="23"/>
       <c r="K90" s="24"/>
       <c r="L90" s="11"/>
       <c r="M90" s="16"/>
@@ -3794,13 +3760,13 @@
       </c>
       <c r="B91" s="11"/>
       <c r="C91" s="21"/>
-      <c r="D91" s="30"/>
+      <c r="D91" s="35"/>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
       <c r="G91" s="27"/>
-      <c r="H91" s="40"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="10"/>
+      <c r="H91" s="30"/>
+      <c r="I91" s="41"/>
+      <c r="J91" s="23"/>
       <c r="K91" s="24"/>
       <c r="L91" s="11"/>
       <c r="M91" s="16"/>
@@ -3812,13 +3778,13 @@
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="21"/>
-      <c r="D92" s="30"/>
+      <c r="D92" s="35"/>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
       <c r="G92" s="28"/>
-      <c r="H92" s="40"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="10"/>
+      <c r="H92" s="30"/>
+      <c r="I92" s="41"/>
+      <c r="J92" s="23"/>
       <c r="K92" s="24"/>
       <c r="L92" s="11"/>
       <c r="M92" s="16"/>
@@ -3830,13 +3796,13 @@
       </c>
       <c r="B93" s="11"/>
       <c r="C93" s="21"/>
-      <c r="D93" s="30"/>
+      <c r="D93" s="35"/>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
       <c r="G93" s="27"/>
-      <c r="H93" s="40"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="10"/>
+      <c r="H93" s="30"/>
+      <c r="I93" s="41"/>
+      <c r="J93" s="23"/>
       <c r="K93" s="24"/>
       <c r="L93" s="11"/>
       <c r="M93" s="16"/>
@@ -3848,13 +3814,13 @@
       </c>
       <c r="B94" s="11"/>
       <c r="C94" s="21"/>
-      <c r="D94" s="30"/>
+      <c r="D94" s="35"/>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
       <c r="G94" s="27"/>
-      <c r="H94" s="40"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="10"/>
+      <c r="H94" s="30"/>
+      <c r="I94" s="41"/>
+      <c r="J94" s="23"/>
       <c r="K94" s="24"/>
       <c r="L94" s="11"/>
       <c r="M94" s="16"/>
@@ -3866,13 +3832,13 @@
       </c>
       <c r="B95" s="11"/>
       <c r="C95" s="21"/>
-      <c r="D95" s="30"/>
+      <c r="D95" s="35"/>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
       <c r="G95" s="26"/>
-      <c r="H95" s="40"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="10"/>
+      <c r="H95" s="30"/>
+      <c r="I95" s="41"/>
+      <c r="J95" s="23"/>
       <c r="K95" s="24"/>
       <c r="L95" s="11"/>
       <c r="M95" s="16"/>
@@ -3884,13 +3850,13 @@
       </c>
       <c r="B96" s="11"/>
       <c r="C96" s="21"/>
-      <c r="D96" s="30"/>
+      <c r="D96" s="35"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
       <c r="G96" s="26"/>
-      <c r="H96" s="40"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="10"/>
+      <c r="H96" s="30"/>
+      <c r="I96" s="41"/>
+      <c r="J96" s="23"/>
       <c r="K96" s="24"/>
       <c r="L96" s="11"/>
       <c r="M96" s="16"/>
@@ -3902,13 +3868,13 @@
       </c>
       <c r="B97" s="11"/>
       <c r="C97" s="21"/>
-      <c r="D97" s="30"/>
+      <c r="D97" s="35"/>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
       <c r="G97" s="26"/>
-      <c r="H97" s="40"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="10"/>
+      <c r="H97" s="30"/>
+      <c r="I97" s="41"/>
+      <c r="J97" s="23"/>
       <c r="K97" s="24"/>
       <c r="L97" s="11"/>
       <c r="M97" s="16"/>
@@ -3920,13 +3886,13 @@
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="21"/>
-      <c r="D98" s="30"/>
+      <c r="D98" s="35"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
       <c r="G98" s="26"/>
-      <c r="H98" s="40"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="10"/>
+      <c r="H98" s="30"/>
+      <c r="I98" s="41"/>
+      <c r="J98" s="23"/>
       <c r="K98" s="24"/>
       <c r="L98" s="11"/>
       <c r="M98" s="16"/>
@@ -3938,13 +3904,13 @@
       </c>
       <c r="B99" s="11"/>
       <c r="C99" s="21"/>
-      <c r="D99" s="30"/>
+      <c r="D99" s="35"/>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
       <c r="G99" s="26"/>
-      <c r="H99" s="40"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="10"/>
+      <c r="H99" s="30"/>
+      <c r="I99" s="41"/>
+      <c r="J99" s="23"/>
       <c r="K99" s="24"/>
       <c r="L99" s="11"/>
       <c r="M99" s="16"/>
@@ -3956,13 +3922,13 @@
       </c>
       <c r="B100" s="11"/>
       <c r="C100" s="21"/>
-      <c r="D100" s="30"/>
+      <c r="D100" s="35"/>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
       <c r="G100" s="26"/>
-      <c r="H100" s="40"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="10"/>
+      <c r="H100" s="30"/>
+      <c r="I100" s="41"/>
+      <c r="J100" s="23"/>
       <c r="K100" s="24"/>
       <c r="L100" s="11"/>
       <c r="M100" s="16"/>
@@ -3974,13 +3940,13 @@
       </c>
       <c r="B101" s="11"/>
       <c r="C101" s="21"/>
-      <c r="D101" s="30"/>
+      <c r="D101" s="35"/>
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
       <c r="G101" s="26"/>
-      <c r="H101" s="40"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="10"/>
+      <c r="H101" s="30"/>
+      <c r="I101" s="41"/>
+      <c r="J101" s="23"/>
       <c r="K101" s="24"/>
       <c r="L101" s="11"/>
       <c r="M101" s="16"/>
@@ -3992,13 +3958,13 @@
       </c>
       <c r="B102" s="11"/>
       <c r="C102" s="21"/>
-      <c r="D102" s="30"/>
+      <c r="D102" s="35"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
       <c r="G102" s="26"/>
-      <c r="H102" s="40"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="10"/>
+      <c r="H102" s="30"/>
+      <c r="I102" s="41"/>
+      <c r="J102" s="23"/>
       <c r="K102" s="24"/>
       <c r="L102" s="11"/>
       <c r="M102" s="16"/>
@@ -4010,13 +3976,13 @@
       </c>
       <c r="B103" s="11"/>
       <c r="C103" s="21"/>
-      <c r="D103" s="30"/>
+      <c r="D103" s="35"/>
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
       <c r="G103" s="26"/>
-      <c r="H103" s="40"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="10"/>
+      <c r="H103" s="30"/>
+      <c r="I103" s="41"/>
+      <c r="J103" s="23"/>
       <c r="K103" s="24"/>
       <c r="L103" s="11"/>
       <c r="M103" s="16"/>
@@ -4028,13 +3994,13 @@
       </c>
       <c r="B104" s="13"/>
       <c r="C104" s="22"/>
-      <c r="D104" s="34"/>
-      <c r="E104" s="35"/>
-      <c r="F104" s="35"/>
-      <c r="G104" s="37"/>
-      <c r="H104" s="41"/>
-      <c r="I104" s="35"/>
-      <c r="J104" s="13"/>
+      <c r="D104" s="36"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="22"/>
+      <c r="H104" s="33"/>
+      <c r="I104" s="42"/>
+      <c r="J104" s="25"/>
       <c r="K104" s="25"/>
       <c r="L104" s="13"/>
       <c r="M104" s="17"/>
@@ -4657,7 +4623,7 @@
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>Index!$A$2:$A$97</xm:f>
@@ -4667,17 +4633,11 @@
           </x14:formula2>
           <xm:sqref>E9:E104 C9:C104 I9:I104</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3A3D75E0-B2D8-5742-9137-9F5386AD1817}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE811C6F-3DAF-FF46-829C-068B224B4727}">
           <x14:formula1>
-            <xm:f>Index!$C$2:$C$14</xm:f>
+            <xm:f>Index!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G9:G63 G95:G103</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{22423519-D6D5-5D42-A4E9-F0EDC60614CE}">
-          <x14:formula1>
-            <xm:f>Index!$C$2:$C$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>G104</xm:sqref>
+          <xm:sqref>G9:G104</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4690,7 +4650,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4718,7 +4678,7 @@
       <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>401</v>
       </c>
     </row>
@@ -4729,7 +4689,7 @@
       <c r="B3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="15" t="s">
         <v>402</v>
       </c>
     </row>
@@ -4740,7 +4700,7 @@
       <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="15" t="s">
         <v>403</v>
       </c>
     </row>
@@ -4751,9 +4711,7 @@
       <c r="B5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>404</v>
-      </c>
+      <c r="C5" s="18"/>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -4762,9 +4720,7 @@
       <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="19" t="s">
-        <v>405</v>
-      </c>
+      <c r="C6" s="19"/>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
@@ -4773,9 +4729,7 @@
       <c r="B7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>406</v>
-      </c>
+      <c r="C7" s="18"/>
     </row>
     <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
@@ -4784,9 +4738,7 @@
       <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="18" t="s">
-        <v>407</v>
-      </c>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
@@ -4795,9 +4747,7 @@
       <c r="B9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>408</v>
-      </c>
+      <c r="C9" s="18"/>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
@@ -4806,9 +4756,7 @@
       <c r="B10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>409</v>
-      </c>
+      <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
@@ -4817,9 +4765,7 @@
       <c r="B11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>410</v>
-      </c>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
@@ -4828,9 +4774,7 @@
       <c r="B12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>411</v>
-      </c>
+      <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
@@ -4839,9 +4783,7 @@
       <c r="B13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>412</v>
-      </c>
+      <c r="C13" s="19"/>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
@@ -4850,9 +4792,7 @@
       <c r="B14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19" t="s">
-        <v>413</v>
-      </c>
+      <c r="C14" s="19"/>
     </row>
     <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">

</xml_diff>